<commit_message>
fix database and features
</commit_message>
<xml_diff>
--- a/public/assets/template/dataset-ticket.xlsx
+++ b/public/assets/template/dataset-ticket.xlsx
@@ -24,38 +24,14 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="34">
-  <si>
-    <t>Urgent</t>
-  </si>
-  <si>
-    <t>Hardware</t>
-  </si>
-  <si>
-    <t>Technical</t>
-  </si>
-  <si>
-    <t>Less Urgent</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="18">
   <si>
     <t>Internet</t>
   </si>
   <si>
-    <t>Generally</t>
-  </si>
-  <si>
     <t>Software</t>
   </si>
   <si>
-    <t>Jaringan Internet</t>
-  </si>
-  <si>
-    <t>Very Urgent</t>
-  </si>
-  <si>
-    <t>Printer</t>
-  </si>
-  <si>
     <t>Staff IT</t>
   </si>
   <si>
@@ -71,61 +47,37 @@
     <t>priority</t>
   </si>
   <si>
-    <t>type</t>
-  </si>
-  <si>
     <t>category</t>
   </si>
   <si>
-    <t>Printer tidak bisa mencetak</t>
-  </si>
-  <si>
-    <t>Printer di ruang kelas X tidak bisa mencetak. Saat dihidupkan, lampu indikator menyala hijau, tetapi tidak ada hasil cetakan yang keluar.</t>
-  </si>
-  <si>
-    <t>Staff TU</t>
-  </si>
-  <si>
-    <t>Jaringan internet tidak stabil</t>
-  </si>
-  <si>
-    <t>Jaringan internet di sekolah sering mengalami gangguan. Saat ini, jaringan internet di ruang guru tidak bisa digunakan untuk mengakses internet.</t>
-  </si>
-  <si>
-    <t>Website sekolah tidak bisa dibuka</t>
-  </si>
-  <si>
-    <t>Website sekolah tidak bisa dibuka. Saat diakses, muncul pesan error "404 Not Found".</t>
-  </si>
-  <si>
     <t>Website</t>
   </si>
   <si>
-    <t>Pembayaran SPP Tidak Terrekam dengan Baik</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Pembayaran SPP siswa tidak terrekam dengan baik oleh sistem keuangan. Siswa diingatkan untuk segera melunasi, padahal pembayaran sudah dilakukan.</t>
-  </si>
-  <si>
-    <t>Keuangan</t>
-  </si>
-  <si>
-    <t>Pembayaran</t>
-  </si>
-  <si>
-    <t>Perpustakaan kurang lengkap</t>
-  </si>
-  <si>
-    <t>Koleksi buku di perpustakaan kurang lengkap. Banyak buku yang sudah usang dan tidak layak baca.</t>
-  </si>
-  <si>
-    <t>Akademik</t>
-  </si>
-  <si>
-    <t>Buku</t>
-  </si>
-  <si>
-    <t>Perpustakaan</t>
+    <t>Microsoft Word Bermasalah</t>
+  </si>
+  <si>
+    <t>microsoft word tidak bisa di ketik</t>
+  </si>
+  <si>
+    <t>Masalah Koneksi Internet</t>
+  </si>
+  <si>
+    <t>Saya mengalami kesulitan untuk terhubung ke internet di ruang kelas A. Sinyal Wi-Fi sangat lemah, dan sering terputus.</t>
+  </si>
+  <si>
+    <t>Tidak Bisa Mengakses Platform E-Learning</t>
+  </si>
+  <si>
+    <t>Saya tidak dapat mengakses platform e-learning. Setiap kali mencoba masuk, halaman web tidak merespons.</t>
+  </si>
+  <si>
+    <t>Low</t>
+  </si>
+  <si>
+    <t>High</t>
+  </si>
+  <si>
+    <t>Administrator</t>
   </si>
 </sst>
 </file>
@@ -449,156 +401,138 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F11"/>
+  <dimension ref="A1:E14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="26.140625" style="2" customWidth="1"/>
-    <col min="2" max="2" width="89" style="2" customWidth="1"/>
-    <col min="3" max="3" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="41.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="107.5703125" style="2" customWidth="1"/>
+    <col min="3" max="3" width="19.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.28515625" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>11</v>
+        <v>3</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="C1" t="s">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="1" t="s">
         <v>15</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>0</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="F2" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>21</v>
+    </row>
+    <row r="3" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" t="s">
+        <v>12</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="D3" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E4" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E3" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="F6" s="1" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5"/>
+      <c r="B5"/>
+      <c r="C5" s="1"/>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6"/>
+      <c r="B6"/>
+      <c r="C6" s="1"/>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7"/>
+      <c r="B7"/>
       <c r="C7" s="1"/>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8"/>
+      <c r="B8"/>
       <c r="C8" s="1"/>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9"/>
+      <c r="B9"/>
       <c r="C9" s="1"/>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10"/>
+      <c r="B10"/>
       <c r="C10" s="1"/>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11"/>
+      <c r="B11"/>
       <c r="C11" s="1"/>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12"/>
+      <c r="B12"/>
+      <c r="C12" s="1"/>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13"/>
+      <c r="B13"/>
+      <c r="C13" s="1"/>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14"/>
+      <c r="B14"/>
+      <c r="C14" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
fix dataset view and added export feature
</commit_message>
<xml_diff>
--- a/public/assets/template/dataset-ticket.xlsx
+++ b/public/assets/template/dataset-ticket.xlsx
@@ -35,24 +35,6 @@
     <t>Staff IT</t>
   </si>
   <si>
-    <t>subject</t>
-  </si>
-  <si>
-    <t>details</t>
-  </si>
-  <si>
-    <t>department</t>
-  </si>
-  <si>
-    <t>priority</t>
-  </si>
-  <si>
-    <t>category</t>
-  </si>
-  <si>
-    <t>Website</t>
-  </si>
-  <si>
     <t>Microsoft Word Bermasalah</t>
   </si>
   <si>
@@ -77,16 +59,42 @@
     <t>High</t>
   </si>
   <si>
-    <t>Administrator</t>
+    <t>Normal</t>
+  </si>
+  <si>
+    <t>E-Learning</t>
+  </si>
+  <si>
+    <t>Subject</t>
+  </si>
+  <si>
+    <t>Details</t>
+  </si>
+  <si>
+    <t>Department</t>
+  </si>
+  <si>
+    <t>Priority</t>
+  </si>
+  <si>
+    <t>Category</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -113,14 +121,21 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -401,138 +416,821 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E14"/>
+  <dimension ref="A1:E111"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="41.85546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="107.5703125" style="2" customWidth="1"/>
-    <col min="3" max="3" width="19.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="45.5703125" style="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="255.7109375" style="4" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.42578125" style="3" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="24.140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="6" max="16384" width="9.140625" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:5" s="1" customFormat="1" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C2" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="B3" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="C3" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B2" t="s">
+      <c r="B4" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D4" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="C2" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>11</v>
-      </c>
-      <c r="B3" t="s">
+      <c r="E4" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="C3" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>13</v>
-      </c>
-      <c r="B4" t="s">
-        <v>14</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5"/>
-      <c r="B5"/>
-      <c r="C5" s="1"/>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6"/>
-      <c r="B6"/>
-      <c r="C6" s="1"/>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7"/>
-      <c r="B7"/>
-      <c r="C7" s="1"/>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8"/>
-      <c r="B8"/>
-      <c r="C8" s="1"/>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9"/>
-      <c r="B9"/>
-      <c r="C9" s="1"/>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10"/>
-      <c r="B10"/>
-      <c r="C10" s="1"/>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11"/>
-      <c r="B11"/>
-      <c r="C11" s="1"/>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12"/>
-      <c r="B12"/>
-      <c r="C12" s="1"/>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13"/>
-      <c r="B13"/>
-      <c r="C13" s="1"/>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14"/>
-      <c r="B14"/>
-      <c r="C14" s="1"/>
+    </row>
+    <row r="5" spans="1:5" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C5" s="3"/>
+      <c r="D5" s="3"/>
+      <c r="E5" s="3"/>
+    </row>
+    <row r="6" spans="1:5" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C6" s="3"/>
+      <c r="D6" s="3"/>
+      <c r="E6" s="3"/>
+    </row>
+    <row r="7" spans="1:5" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C7" s="3"/>
+      <c r="D7" s="3"/>
+      <c r="E7" s="3"/>
+    </row>
+    <row r="8" spans="1:5" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C8" s="3"/>
+      <c r="D8" s="3"/>
+      <c r="E8" s="3"/>
+    </row>
+    <row r="9" spans="1:5" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C9" s="3"/>
+      <c r="D9" s="3"/>
+      <c r="E9" s="3"/>
+    </row>
+    <row r="10" spans="1:5" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C10" s="3"/>
+      <c r="D10" s="3"/>
+      <c r="E10" s="3"/>
+    </row>
+    <row r="11" spans="1:5" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C11" s="3"/>
+      <c r="D11" s="3"/>
+      <c r="E11" s="3"/>
+    </row>
+    <row r="12" spans="1:5" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C12" s="3"/>
+      <c r="D12" s="3"/>
+      <c r="E12" s="3"/>
+    </row>
+    <row r="13" spans="1:5" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B13" s="4"/>
+      <c r="C13" s="3"/>
+      <c r="D13" s="3"/>
+      <c r="E13" s="3"/>
+    </row>
+    <row r="14" spans="1:5" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="4"/>
+      <c r="B14" s="4"/>
+      <c r="C14" s="3"/>
+      <c r="D14" s="3"/>
+      <c r="E14" s="3"/>
+    </row>
+    <row r="15" spans="1:5" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="4"/>
+      <c r="B15" s="4"/>
+      <c r="C15" s="3"/>
+      <c r="D15" s="3"/>
+      <c r="E15" s="3"/>
+    </row>
+    <row r="16" spans="1:5" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="4"/>
+      <c r="B16" s="4"/>
+      <c r="C16" s="3"/>
+      <c r="D16" s="3"/>
+      <c r="E16" s="3"/>
+    </row>
+    <row r="17" spans="1:5" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="4"/>
+      <c r="B17" s="4"/>
+      <c r="C17" s="3"/>
+      <c r="D17" s="3"/>
+      <c r="E17" s="3"/>
+    </row>
+    <row r="18" spans="1:5" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="4"/>
+      <c r="B18" s="4"/>
+      <c r="C18" s="3"/>
+      <c r="D18" s="3"/>
+      <c r="E18" s="3"/>
+    </row>
+    <row r="19" spans="1:5" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="4"/>
+      <c r="B19" s="4"/>
+      <c r="C19" s="3"/>
+      <c r="D19" s="3"/>
+      <c r="E19" s="3"/>
+    </row>
+    <row r="20" spans="1:5" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="4"/>
+      <c r="B20" s="4"/>
+      <c r="C20" s="3"/>
+      <c r="D20" s="3"/>
+      <c r="E20" s="3"/>
+    </row>
+    <row r="21" spans="1:5" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="4"/>
+      <c r="B21" s="4"/>
+      <c r="C21" s="3"/>
+      <c r="D21" s="3"/>
+      <c r="E21" s="3"/>
+    </row>
+    <row r="22" spans="1:5" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="4"/>
+      <c r="B22" s="4"/>
+      <c r="C22" s="3"/>
+      <c r="D22" s="3"/>
+      <c r="E22" s="3"/>
+    </row>
+    <row r="23" spans="1:5" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="4"/>
+      <c r="B23" s="4"/>
+      <c r="C23" s="3"/>
+      <c r="D23" s="3"/>
+      <c r="E23" s="3"/>
+    </row>
+    <row r="24" spans="1:5" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="4"/>
+      <c r="B24" s="4"/>
+      <c r="C24" s="3"/>
+      <c r="D24" s="3"/>
+      <c r="E24" s="3"/>
+    </row>
+    <row r="25" spans="1:5" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="4"/>
+      <c r="B25" s="4"/>
+      <c r="C25" s="3"/>
+      <c r="D25" s="3"/>
+      <c r="E25" s="3"/>
+    </row>
+    <row r="26" spans="1:5" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="4"/>
+      <c r="B26" s="4"/>
+      <c r="C26" s="3"/>
+      <c r="D26" s="3"/>
+      <c r="E26" s="3"/>
+    </row>
+    <row r="27" spans="1:5" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="4"/>
+      <c r="B27" s="4"/>
+      <c r="C27" s="3"/>
+      <c r="D27" s="3"/>
+      <c r="E27" s="3"/>
+    </row>
+    <row r="28" spans="1:5" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="4"/>
+      <c r="B28" s="4"/>
+      <c r="C28" s="3"/>
+      <c r="D28" s="3"/>
+      <c r="E28" s="3"/>
+    </row>
+    <row r="29" spans="1:5" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="4"/>
+      <c r="B29" s="4"/>
+      <c r="C29" s="3"/>
+      <c r="D29" s="3"/>
+      <c r="E29" s="3"/>
+    </row>
+    <row r="30" spans="1:5" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="4"/>
+      <c r="B30" s="4"/>
+      <c r="C30" s="3"/>
+      <c r="D30" s="3"/>
+      <c r="E30" s="3"/>
+    </row>
+    <row r="31" spans="1:5" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="4"/>
+      <c r="B31" s="4"/>
+      <c r="C31" s="3"/>
+      <c r="D31" s="3"/>
+      <c r="E31" s="3"/>
+    </row>
+    <row r="32" spans="1:5" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="4"/>
+      <c r="B32" s="4"/>
+      <c r="C32" s="3"/>
+      <c r="D32" s="3"/>
+      <c r="E32" s="3"/>
+    </row>
+    <row r="33" spans="1:5" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="4"/>
+      <c r="B33" s="4"/>
+      <c r="C33" s="3"/>
+      <c r="D33" s="3"/>
+      <c r="E33" s="3"/>
+    </row>
+    <row r="34" spans="1:5" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="4"/>
+      <c r="B34" s="4"/>
+      <c r="C34" s="3"/>
+      <c r="D34" s="3"/>
+      <c r="E34" s="3"/>
+    </row>
+    <row r="35" spans="1:5" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="4"/>
+      <c r="B35" s="4"/>
+      <c r="C35" s="3"/>
+      <c r="D35" s="3"/>
+      <c r="E35" s="3"/>
+    </row>
+    <row r="36" spans="1:5" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="4"/>
+      <c r="B36" s="4"/>
+      <c r="C36" s="3"/>
+      <c r="D36" s="3"/>
+      <c r="E36" s="3"/>
+    </row>
+    <row r="37" spans="1:5" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="4"/>
+      <c r="B37" s="4"/>
+      <c r="C37" s="3"/>
+      <c r="D37" s="3"/>
+      <c r="E37" s="3"/>
+    </row>
+    <row r="38" spans="1:5" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="4"/>
+      <c r="B38" s="4"/>
+      <c r="C38" s="3"/>
+      <c r="D38" s="3"/>
+      <c r="E38" s="3"/>
+    </row>
+    <row r="39" spans="1:5" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="4"/>
+      <c r="B39" s="4"/>
+      <c r="C39" s="3"/>
+      <c r="D39" s="3"/>
+      <c r="E39" s="3"/>
+    </row>
+    <row r="40" spans="1:5" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="4"/>
+      <c r="B40" s="4"/>
+      <c r="C40" s="3"/>
+      <c r="D40" s="3"/>
+      <c r="E40" s="3"/>
+    </row>
+    <row r="41" spans="1:5" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="4"/>
+      <c r="B41" s="4"/>
+      <c r="C41" s="3"/>
+      <c r="D41" s="3"/>
+      <c r="E41" s="3"/>
+    </row>
+    <row r="42" spans="1:5" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="4"/>
+      <c r="B42" s="4"/>
+      <c r="C42" s="3"/>
+      <c r="D42" s="3"/>
+      <c r="E42" s="3"/>
+    </row>
+    <row r="43" spans="1:5" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="4"/>
+      <c r="B43" s="4"/>
+      <c r="C43" s="3"/>
+      <c r="D43" s="3"/>
+      <c r="E43" s="3"/>
+    </row>
+    <row r="44" spans="1:5" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A44" s="4"/>
+      <c r="B44" s="4"/>
+      <c r="C44" s="3"/>
+      <c r="D44" s="3"/>
+      <c r="E44" s="3"/>
+    </row>
+    <row r="45" spans="1:5" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A45" s="4"/>
+      <c r="B45" s="4"/>
+      <c r="C45" s="3"/>
+      <c r="D45" s="3"/>
+      <c r="E45" s="3"/>
+    </row>
+    <row r="46" spans="1:5" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A46" s="4"/>
+      <c r="B46" s="4"/>
+      <c r="C46" s="3"/>
+      <c r="D46" s="3"/>
+      <c r="E46" s="3"/>
+    </row>
+    <row r="47" spans="1:5" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A47" s="4"/>
+      <c r="B47" s="4"/>
+      <c r="C47" s="3"/>
+      <c r="D47" s="3"/>
+      <c r="E47" s="3"/>
+    </row>
+    <row r="48" spans="1:5" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A48" s="4"/>
+      <c r="B48" s="4"/>
+      <c r="C48" s="3"/>
+      <c r="D48" s="3"/>
+      <c r="E48" s="3"/>
+    </row>
+    <row r="49" spans="1:5" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A49" s="4"/>
+      <c r="B49" s="4"/>
+      <c r="C49" s="3"/>
+      <c r="D49" s="3"/>
+      <c r="E49" s="3"/>
+    </row>
+    <row r="50" spans="1:5" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A50" s="4"/>
+      <c r="B50" s="4"/>
+      <c r="C50" s="3"/>
+      <c r="D50" s="3"/>
+      <c r="E50" s="3"/>
+    </row>
+    <row r="51" spans="1:5" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A51" s="4"/>
+      <c r="B51" s="4"/>
+      <c r="C51" s="3"/>
+      <c r="D51" s="3"/>
+      <c r="E51" s="3"/>
+    </row>
+    <row r="52" spans="1:5" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A52" s="4"/>
+      <c r="B52" s="4"/>
+      <c r="C52" s="3"/>
+      <c r="D52" s="3"/>
+      <c r="E52" s="3"/>
+    </row>
+    <row r="53" spans="1:5" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A53" s="4"/>
+      <c r="B53" s="4"/>
+      <c r="C53" s="3"/>
+      <c r="D53" s="3"/>
+      <c r="E53" s="3"/>
+    </row>
+    <row r="54" spans="1:5" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A54" s="4"/>
+      <c r="B54" s="4"/>
+      <c r="C54" s="3"/>
+      <c r="D54" s="3"/>
+      <c r="E54" s="3"/>
+    </row>
+    <row r="55" spans="1:5" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A55" s="4"/>
+      <c r="B55" s="4"/>
+      <c r="C55" s="3"/>
+      <c r="D55" s="3"/>
+      <c r="E55" s="3"/>
+    </row>
+    <row r="56" spans="1:5" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A56" s="4"/>
+      <c r="B56" s="4"/>
+      <c r="C56" s="3"/>
+      <c r="D56" s="3"/>
+      <c r="E56" s="3"/>
+    </row>
+    <row r="57" spans="1:5" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A57" s="4"/>
+      <c r="B57" s="4"/>
+      <c r="C57" s="3"/>
+      <c r="D57" s="3"/>
+      <c r="E57" s="3"/>
+    </row>
+    <row r="58" spans="1:5" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A58" s="4"/>
+      <c r="B58" s="4"/>
+      <c r="C58" s="3"/>
+      <c r="D58" s="3"/>
+      <c r="E58" s="3"/>
+    </row>
+    <row r="59" spans="1:5" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A59" s="4"/>
+      <c r="B59" s="4"/>
+      <c r="C59" s="3"/>
+      <c r="D59" s="3"/>
+      <c r="E59" s="3"/>
+    </row>
+    <row r="60" spans="1:5" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A60" s="4"/>
+      <c r="B60" s="4"/>
+      <c r="C60" s="3"/>
+      <c r="D60" s="3"/>
+      <c r="E60" s="3"/>
+    </row>
+    <row r="61" spans="1:5" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A61" s="4"/>
+      <c r="B61" s="4"/>
+      <c r="C61" s="3"/>
+      <c r="D61" s="3"/>
+      <c r="E61" s="3"/>
+    </row>
+    <row r="62" spans="1:5" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A62" s="4"/>
+      <c r="B62" s="4"/>
+      <c r="C62" s="3"/>
+      <c r="D62" s="3"/>
+      <c r="E62" s="3"/>
+    </row>
+    <row r="63" spans="1:5" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A63" s="4"/>
+      <c r="B63" s="4"/>
+      <c r="C63" s="3"/>
+      <c r="D63" s="3"/>
+      <c r="E63" s="3"/>
+    </row>
+    <row r="64" spans="1:5" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A64" s="4"/>
+      <c r="B64" s="4"/>
+      <c r="C64" s="3"/>
+      <c r="D64" s="3"/>
+      <c r="E64" s="3"/>
+    </row>
+    <row r="65" spans="1:5" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A65" s="4"/>
+      <c r="B65" s="4"/>
+      <c r="C65" s="3"/>
+      <c r="D65" s="3"/>
+      <c r="E65" s="3"/>
+    </row>
+    <row r="66" spans="1:5" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A66" s="4"/>
+      <c r="B66" s="4"/>
+      <c r="C66" s="3"/>
+      <c r="D66" s="3"/>
+      <c r="E66" s="3"/>
+    </row>
+    <row r="67" spans="1:5" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A67" s="4"/>
+      <c r="B67" s="4"/>
+      <c r="C67" s="3"/>
+      <c r="D67" s="3"/>
+      <c r="E67" s="3"/>
+    </row>
+    <row r="68" spans="1:5" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A68" s="4"/>
+      <c r="B68" s="4"/>
+      <c r="C68" s="3"/>
+      <c r="D68" s="3"/>
+      <c r="E68" s="3"/>
+    </row>
+    <row r="69" spans="1:5" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A69" s="4"/>
+      <c r="B69" s="4"/>
+      <c r="C69" s="3"/>
+      <c r="D69" s="3"/>
+      <c r="E69" s="3"/>
+    </row>
+    <row r="70" spans="1:5" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A70" s="4"/>
+      <c r="B70" s="4"/>
+      <c r="C70" s="3"/>
+      <c r="D70" s="3"/>
+      <c r="E70" s="3"/>
+    </row>
+    <row r="71" spans="1:5" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A71" s="4"/>
+      <c r="B71" s="4"/>
+      <c r="C71" s="3"/>
+      <c r="D71" s="3"/>
+      <c r="E71" s="3"/>
+    </row>
+    <row r="72" spans="1:5" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A72" s="4"/>
+      <c r="B72" s="4"/>
+      <c r="C72" s="3"/>
+      <c r="D72" s="3"/>
+      <c r="E72" s="3"/>
+    </row>
+    <row r="73" spans="1:5" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A73" s="4"/>
+      <c r="B73" s="4"/>
+      <c r="C73" s="3"/>
+      <c r="D73" s="3"/>
+      <c r="E73" s="3"/>
+    </row>
+    <row r="74" spans="1:5" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A74" s="4"/>
+      <c r="B74" s="4"/>
+      <c r="C74" s="3"/>
+      <c r="D74" s="3"/>
+      <c r="E74" s="3"/>
+    </row>
+    <row r="75" spans="1:5" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A75" s="4"/>
+      <c r="B75" s="4"/>
+      <c r="C75" s="3"/>
+      <c r="D75" s="3"/>
+      <c r="E75" s="3"/>
+    </row>
+    <row r="76" spans="1:5" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A76" s="4"/>
+      <c r="B76" s="4"/>
+      <c r="C76" s="3"/>
+      <c r="D76" s="3"/>
+      <c r="E76" s="3"/>
+    </row>
+    <row r="77" spans="1:5" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A77" s="4"/>
+      <c r="B77" s="4"/>
+      <c r="C77" s="3"/>
+      <c r="D77" s="3"/>
+      <c r="E77" s="3"/>
+    </row>
+    <row r="78" spans="1:5" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A78" s="4"/>
+      <c r="B78" s="4"/>
+      <c r="C78" s="3"/>
+      <c r="D78" s="3"/>
+      <c r="E78" s="3"/>
+    </row>
+    <row r="79" spans="1:5" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A79" s="4"/>
+      <c r="B79" s="4"/>
+      <c r="C79" s="3"/>
+      <c r="D79" s="3"/>
+      <c r="E79" s="3"/>
+    </row>
+    <row r="80" spans="1:5" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A80" s="4"/>
+      <c r="B80" s="4"/>
+      <c r="C80" s="3"/>
+      <c r="D80" s="3"/>
+      <c r="E80" s="3"/>
+    </row>
+    <row r="81" spans="1:5" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A81" s="4"/>
+      <c r="B81" s="4"/>
+      <c r="C81" s="3"/>
+      <c r="D81" s="3"/>
+      <c r="E81" s="3"/>
+    </row>
+    <row r="82" spans="1:5" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A82" s="4"/>
+      <c r="B82" s="4"/>
+      <c r="C82" s="3"/>
+      <c r="D82" s="3"/>
+      <c r="E82" s="3"/>
+    </row>
+    <row r="83" spans="1:5" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A83" s="4"/>
+      <c r="B83" s="4"/>
+      <c r="C83" s="3"/>
+      <c r="D83" s="3"/>
+      <c r="E83" s="3"/>
+    </row>
+    <row r="84" spans="1:5" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A84" s="4"/>
+      <c r="B84" s="4"/>
+      <c r="C84" s="3"/>
+      <c r="D84" s="3"/>
+      <c r="E84" s="3"/>
+    </row>
+    <row r="85" spans="1:5" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A85" s="4"/>
+      <c r="B85" s="4"/>
+      <c r="C85" s="3"/>
+      <c r="D85" s="3"/>
+      <c r="E85" s="3"/>
+    </row>
+    <row r="86" spans="1:5" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A86" s="4"/>
+      <c r="B86" s="4"/>
+      <c r="C86" s="3"/>
+      <c r="D86" s="3"/>
+      <c r="E86" s="3"/>
+    </row>
+    <row r="87" spans="1:5" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A87" s="4"/>
+      <c r="B87" s="4"/>
+      <c r="C87" s="3"/>
+      <c r="D87" s="3"/>
+      <c r="E87" s="3"/>
+    </row>
+    <row r="88" spans="1:5" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A88" s="4"/>
+      <c r="B88" s="4"/>
+      <c r="C88" s="3"/>
+      <c r="D88" s="3"/>
+      <c r="E88" s="3"/>
+    </row>
+    <row r="89" spans="1:5" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A89" s="4"/>
+      <c r="B89" s="4"/>
+      <c r="C89" s="3"/>
+      <c r="D89" s="3"/>
+      <c r="E89" s="3"/>
+    </row>
+    <row r="90" spans="1:5" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A90" s="4"/>
+      <c r="B90" s="4"/>
+      <c r="C90" s="3"/>
+      <c r="D90" s="3"/>
+      <c r="E90" s="3"/>
+    </row>
+    <row r="91" spans="1:5" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A91" s="4"/>
+      <c r="B91" s="4"/>
+      <c r="C91" s="3"/>
+      <c r="D91" s="3"/>
+      <c r="E91" s="3"/>
+    </row>
+    <row r="92" spans="1:5" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A92" s="4"/>
+      <c r="B92" s="4"/>
+      <c r="C92" s="3"/>
+      <c r="D92" s="3"/>
+      <c r="E92" s="3"/>
+    </row>
+    <row r="93" spans="1:5" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A93" s="4"/>
+      <c r="B93" s="4"/>
+      <c r="C93" s="3"/>
+      <c r="D93" s="3"/>
+      <c r="E93" s="3"/>
+    </row>
+    <row r="94" spans="1:5" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A94" s="4"/>
+      <c r="B94" s="4"/>
+      <c r="C94" s="3"/>
+      <c r="D94" s="3"/>
+      <c r="E94" s="3"/>
+    </row>
+    <row r="95" spans="1:5" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A95" s="4"/>
+      <c r="B95" s="4"/>
+      <c r="C95" s="3"/>
+      <c r="D95" s="3"/>
+      <c r="E95" s="3"/>
+    </row>
+    <row r="96" spans="1:5" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A96" s="4"/>
+      <c r="B96" s="4"/>
+      <c r="C96" s="3"/>
+      <c r="D96" s="3"/>
+      <c r="E96" s="3"/>
+    </row>
+    <row r="97" spans="1:5" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A97" s="4"/>
+      <c r="B97" s="4"/>
+      <c r="C97" s="3"/>
+      <c r="D97" s="3"/>
+      <c r="E97" s="3"/>
+    </row>
+    <row r="98" spans="1:5" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A98" s="4"/>
+      <c r="B98" s="4"/>
+      <c r="C98" s="3"/>
+      <c r="D98" s="3"/>
+      <c r="E98" s="3"/>
+    </row>
+    <row r="99" spans="1:5" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A99" s="4"/>
+      <c r="B99" s="4"/>
+      <c r="C99" s="3"/>
+      <c r="D99" s="3"/>
+      <c r="E99" s="3"/>
+    </row>
+    <row r="100" spans="1:5" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A100" s="4"/>
+      <c r="B100" s="4"/>
+      <c r="C100" s="3"/>
+      <c r="D100" s="3"/>
+      <c r="E100" s="3"/>
+    </row>
+    <row r="101" spans="1:5" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A101" s="4"/>
+      <c r="B101" s="4"/>
+      <c r="C101" s="3"/>
+      <c r="D101" s="3"/>
+      <c r="E101" s="3"/>
+    </row>
+    <row r="102" spans="1:5" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A102" s="4"/>
+      <c r="B102" s="4"/>
+      <c r="C102" s="3"/>
+      <c r="D102" s="3"/>
+      <c r="E102" s="3"/>
+    </row>
+    <row r="103" spans="1:5" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A103" s="4"/>
+      <c r="B103" s="4"/>
+      <c r="C103" s="3"/>
+      <c r="D103" s="3"/>
+      <c r="E103" s="3"/>
+    </row>
+    <row r="104" spans="1:5" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A104" s="4"/>
+      <c r="B104" s="4"/>
+      <c r="C104" s="3"/>
+      <c r="D104" s="3"/>
+      <c r="E104" s="3"/>
+    </row>
+    <row r="105" spans="1:5" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A105" s="4"/>
+      <c r="B105" s="4"/>
+      <c r="C105" s="3"/>
+      <c r="D105" s="3"/>
+      <c r="E105" s="3"/>
+    </row>
+    <row r="106" spans="1:5" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A106" s="4"/>
+      <c r="B106" s="4"/>
+      <c r="C106" s="3"/>
+      <c r="D106" s="3"/>
+      <c r="E106" s="3"/>
+    </row>
+    <row r="107" spans="1:5" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A107" s="4"/>
+      <c r="B107" s="4"/>
+      <c r="C107" s="3"/>
+      <c r="D107" s="3"/>
+      <c r="E107" s="3"/>
+    </row>
+    <row r="108" spans="1:5" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A108" s="4"/>
+      <c r="B108" s="4"/>
+      <c r="C108" s="3"/>
+      <c r="D108" s="3"/>
+      <c r="E108" s="3"/>
+    </row>
+    <row r="109" spans="1:5" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A109" s="4"/>
+      <c r="B109" s="4"/>
+      <c r="C109" s="3"/>
+      <c r="D109" s="3"/>
+      <c r="E109" s="3"/>
+    </row>
+    <row r="110" spans="1:5" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A110" s="4"/>
+      <c r="B110" s="4"/>
+      <c r="C110" s="3"/>
+      <c r="D110" s="3"/>
+      <c r="E110" s="3"/>
+    </row>
+    <row r="111" spans="1:5" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A111" s="4"/>
+      <c r="B111" s="4"/>
+      <c r="C111" s="3"/>
+      <c r="D111" s="3"/>
+      <c r="E111" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>